<commit_message>
redistributed lab 1 points
</commit_message>
<xml_diff>
--- a/lab1/lab1.xlsx
+++ b/lab1/lab1.xlsx
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>R1-R2, R6-R13, R16</t>
+          <t>R1-R2, R6-R8, R10-R13, R16</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -467,18 +467,18 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1 x 11 = 11 pt(s)</t>
+          <t>1 x 10 = 10 pt(s)</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>R15, R17-R20, R22</t>
+          <t>R9, R17-R20</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -487,18 +487,18 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2 x 6 = 12 pt(s)</t>
+          <t>2 x 5 = 10 pt(s)</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>R3-R5, R21</t>
+          <t>R3, R15, R22</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -507,18 +507,18 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>3 x 4 = 12 pt(s)</t>
+          <t>3 x 3 = 9 pt(s)</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>R14, R23</t>
+          <t>R4-R5, R14, R21, R23</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -527,18 +527,18 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>4 x 2 = 8 pt(s)</t>
+          <t>4 x 5 = 20 pt(s)</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>S1-S9</t>
+          <t>S1-S7</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -547,11 +547,11 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>3 x 9 = 27 pt(s)</t>
+          <t>3 x 7 = 21 pt(s)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
redistributed lab 1 points (fixed)
</commit_message>
<xml_diff>
--- a/lab1/lab1.xlsx
+++ b/lab1/lab1.xlsx
@@ -498,7 +498,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>R3, R15, R22</t>
+          <t>R5, R15, R22</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -518,7 +518,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>R4-R5, R14, R21, R23</t>
+          <t>R3-R4, R14, R21, R23</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">

</xml_diff>